<commit_message>
First draft of input data notebook, including note that describes how to properly read csv and excel files
</commit_message>
<xml_diff>
--- a/docs/examples/data/MFA_modelInputsData/ms_measurement_csv_input_example.xlsx
+++ b/docs/examples/data/MFA_modelInputsData/ms_measurement_csv_input_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s143838/projects/AutoFlow-OmicsDataHandling/docs/examples/data/MFA_modelInputsData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BA41CF-5EEB-5341-B3D6-ADEDCA198CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{951780DC-C1E8-7A49-B207-CC1EAACA42D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{358D565F-7B13-7747-B140-238087DE4E00}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="ms_measurement_csv_input_example" localSheetId="0">Sheet1!$A$1:$H$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{D2277F22-9561-8344-A79C-535A179CC7F5}" name="ms_measurement_csv_input_example" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/s143838/projects/AutoFlow-OmicsDataHandling/docs/examples/data/MFA_modelInputsData/ms_measurement_csv_input_example.csv" thousands="_x0000_" tab="0" comma="1">
+    <textPr sourceFile="/Users/s143838/projects/AutoFlow-OmicsDataHandling/docs/examples/data/MFA_modelInputsData/ms_measurement_csv_input_example.csv" thousands="_x0000_" tab="0" comma="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -105,22 +106,22 @@
     <t>C2H4Si</t>
   </si>
   <si>
-    <t>"[1,2]"</t>
-  </si>
-  <si>
-    <t>"['C3','C4']"</t>
-  </si>
-  <si>
-    <t>"[1.0, 0.4]"</t>
-  </si>
-  <si>
-    <t>"[2.0]"</t>
-  </si>
-  <si>
-    <t>"[0.2]"</t>
-  </si>
-  <si>
-    <t>"[0.1, 0.2]"</t>
+    <t>[1,2]</t>
+  </si>
+  <si>
+    <t>['C3','C4']</t>
+  </si>
+  <si>
+    <t>[1.0, 0.4]</t>
+  </si>
+  <si>
+    <t>[2.0]</t>
+  </si>
+  <si>
+    <t>[0.1, 0.2]</t>
+  </si>
+  <si>
+    <t>[0.2]</t>
   </si>
 </sst>
 </file>
@@ -485,7 +486,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,7 +547,7 @@
         <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -572,7 +573,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3">
         <v>1</v>

</xml_diff>

<commit_message>
MFA input data documentation now utilise a function to present an overview of the data requirements
</commit_message>
<xml_diff>
--- a/docs/examples/data/MFA_modelInputsData/ms_measurement_csv_input_example.xlsx
+++ b/docs/examples/data/MFA_modelInputsData/ms_measurement_csv_input_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s143838/projects/AutoFlow-OmicsDataHandling/docs/examples/data/MFA_modelInputsData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{951780DC-C1E8-7A49-B207-CC1EAACA42D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB264C1B-6E76-B24B-BF06-E47416A0B1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{358D565F-7B13-7747-B140-238087DE4E00}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="68800" windowHeight="28800" xr2:uid="{358D565F-7B13-7747-B140-238087DE4E00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>experiment_id</t>
   </si>
@@ -76,59 +76,62 @@
     <t>unlabelled_atoms</t>
   </si>
   <si>
-    <t>idv</t>
-  </si>
-  <si>
-    <t>idv_std_error</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
     <t>exp1</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>A_260</t>
-  </si>
-  <si>
-    <t>C7H19O</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>B_381</t>
-  </si>
-  <si>
-    <t>C2H4Si</t>
-  </si>
-  <si>
-    <t>[1,2]</t>
-  </si>
-  <si>
-    <t>['C3','C4']</t>
-  </si>
-  <si>
-    <t>[1.0, 0.4]</t>
-  </si>
-  <si>
-    <t>[2.0]</t>
-  </si>
-  <si>
-    <t>[0.1, 0.2]</t>
-  </si>
-  <si>
-    <t>[0.2]</t>
+    <t>measurement_replicate</t>
+  </si>
+  <si>
+    <t>mass_isotope</t>
+  </si>
+  <si>
+    <t>intensity</t>
+  </si>
+  <si>
+    <t>intensity_std_error</t>
+  </si>
+  <si>
+    <t>tyr</t>
+  </si>
+  <si>
+    <t>tyr_302</t>
+  </si>
+  <si>
+    <t>[1, 2]</t>
+  </si>
+  <si>
+    <t>C12H32O2NSi2</t>
+  </si>
+  <si>
+    <t>ser</t>
+  </si>
+  <si>
+    <t>ser_390</t>
+  </si>
+  <si>
+    <t>[1, 2, 3]</t>
+  </si>
+  <si>
+    <t>C14H40O3NSi3</t>
+  </si>
+  <si>
+    <t>ser_362</t>
+  </si>
+  <si>
+    <t>[2, 3]</t>
+  </si>
+  <si>
+    <t>C14H40O2NSi3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,8 +140,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <name val="Menlo"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -162,9 +173,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F7DD57-11BC-A148-AE84-8C8D38A82291}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,82 +513,356 @@
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I7" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H3">
-        <v>1</v>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>